<commit_message>
Comment for AICK: Split of AFASpectra and reduction to max 2048 bytes
</commit_message>
<xml_diff>
--- a/src/fpgaPlayground/HLS/AFAalpha/resources/AFASpectraCalculations.xlsx
+++ b/src/fpgaPlayground/HLS/AFAalpha/resources/AFASpectraCalculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>numSamplesBOSS</t>
   </si>
@@ -87,6 +87,30 @@
   </si>
   <si>
     <t>char</t>
+  </si>
+  <si>
+    <t>numSamplesSDSS</t>
+  </si>
+  <si>
+    <t>which?</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>TypeSize</t>
+  </si>
+  <si>
+    <t>NumOf</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -404,40 +428,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F19"/>
+  <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="14.9453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.68359375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4700</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="F6">
-        <f>ROUNDDOWN(F4/F5,0)</f>
-        <v>587</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6">
+        <f>ROUNDDOWN(INDEX(G3:G4,G2,1)/G5,0)</f>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -448,15 +516,18 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <f>F6</f>
-        <v>587</v>
-      </c>
-      <c r="F9">
-        <f>D9*E9</f>
-        <v>2348</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <f>G6</f>
+        <v>487</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>IF(F9,D9*E9,0)</f>
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -469,8 +540,15 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G19" si="0">IF(F10,D10*E10,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -483,8 +561,15 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -497,8 +582,15 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -511,8 +603,15 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -525,8 +624,15 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -539,19 +645,36 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -564,8 +687,15 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -578,8 +708,15 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -591,6 +728,19 @@
       </c>
       <c r="E19">
         <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21">
+        <f>SUM(G9:G19)</f>
+        <v>1968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>